<commit_message>
Deleted many outdated results from figures directory
</commit_message>
<xml_diff>
--- a/figures/Combination with PCA and Lin Strats.xlsx
+++ b/figures/Combination with PCA and Lin Strats.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,6 +449,17 @@
           <t>PCA Step 1 and Lin Step 1</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>62.47613131263947</v>
+      </c>
+      <c r="C2">
+        <f>AVERAGE(B2:B2)</f>
+        <v/>
+      </c>
+      <c r="D2">
+        <f>STDEV(B2:B2)</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -456,6 +467,17 @@
           <t>PCA Step 1 and Lin Step 3</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>66.53155233183062</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(B3:B3)</f>
+        <v/>
+      </c>
+      <c r="D3">
+        <f>STDEV(B3:B3)</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -463,6 +485,17 @@
           <t>PCA Step 1 and Lin Step 5</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>68.77501848443904</v>
+      </c>
+      <c r="C4">
+        <f>AVERAGE(B4:B4)</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>STDEV(B4:B4)</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -470,6 +503,17 @@
           <t>PCA Step 3 and Lin Step 1</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>69.39889936748489</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGE(B5:B5)</f>
+        <v/>
+      </c>
+      <c r="D5">
+        <f>STDEV(B5:B5)</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -477,6 +521,17 @@
           <t>PCA Step 3 and Lin Step 3</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>75.54199288655842</v>
+      </c>
+      <c r="C6">
+        <f>AVERAGE(B6:B6)</f>
+        <v/>
+      </c>
+      <c r="D6">
+        <f>STDEV(B6:B6)</f>
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -484,12 +539,34 @@
           <t>PCA Step 3 and Lin Step 5</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>74.5336110899503</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(B7:B7)</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>STDEV(B7:B7)</f>
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>PCA Step 5 and Lin Step 1</t>
         </is>
+      </c>
+      <c r="B8" t="n">
+        <v>71.88476462614811</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(B8:B8)</f>
+        <v/>
+      </c>
+      <c r="D8">
+        <f>STDEV(B8:B8)</f>
+        <v/>
       </c>
     </row>
     <row r="9">

</xml_diff>